<commit_message>
11/5 site qltsdemo Pass login, allocation
</commit_message>
<xml_diff>
--- a/File/Mẫu nhập tài sản đã cấp phát.xlsx
+++ b/File/Mẫu nhập tài sản đã cấp phát.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="84">
   <si>
     <t>ma_phong_ban</t>
   </si>
@@ -300,6 +300,42 @@
   </si>
   <si>
     <t>04/05/2025</t>
+  </si>
+  <si>
+    <t>TS-007845</t>
+  </si>
+  <si>
+    <t>TS-007894</t>
+  </si>
+  <si>
+    <t>KTS-MOI</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>23/09/2024</t>
+  </si>
+  <si>
+    <t>sondt</t>
+  </si>
+  <si>
+    <t>22/09/2024</t>
+  </si>
+  <si>
+    <t>21/09/2024</t>
+  </si>
+  <si>
+    <t>TS-007871</t>
+  </si>
+  <si>
+    <t>KTS-TAM</t>
+  </si>
+  <si>
+    <t>20/09/2024</t>
+  </si>
+  <si>
+    <t>K.CCDC</t>
   </si>
 </sst>
 </file>
@@ -876,16 +912,16 @@
         <v>45</v>
       </c>
       <c r="B6" t="s" s="15">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="C6" t="s" s="14">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s" s="23">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="E6" t="s" s="14">
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sua CI chay TestNG, them test Bao mat, hieu nang
</commit_message>
<xml_diff>
--- a/File/Mẫu nhập tài sản đã cấp phát.xlsx
+++ b/File/Mẫu nhập tài sản đã cấp phát.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="86">
   <si>
     <t>ma_phong_ban</t>
   </si>
@@ -336,6 +336,12 @@
   </si>
   <si>
     <t>K.CCDC</t>
+  </si>
+  <si>
+    <t>15/05/2025</t>
+  </si>
+  <si>
+    <t>TS-007502</t>
   </si>
 </sst>
 </file>
@@ -912,13 +918,13 @@
         <v>45</v>
       </c>
       <c r="B6" t="s" s="15">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s" s="14">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="D6" t="s" s="23">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E6" t="s" s="14">
         <v>75</v>

</xml_diff>

<commit_message>
18/5 ( chua co: maintain App + api + tranfer luong)
</commit_message>
<xml_diff>
--- a/File/Mẫu nhập tài sản đã cấp phát.xlsx
+++ b/File/Mẫu nhập tài sản đã cấp phát.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="74">
   <si>
     <t>ma_phong_ban</t>
   </si>
@@ -257,91 +257,55 @@
     <t>Ghi chú 2</t>
   </si>
   <si>
-    <t>27/11/2024</t>
-  </si>
-  <si>
-    <t>TS-007856</t>
-  </si>
-  <si>
-    <t>KT001</t>
-  </si>
-  <si>
-    <t>4.3.KXN</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>TS-007855</t>
+    <t>TS-007100</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>01/08/2024</t>
   </si>
   <si>
     <t>29/02/2025</t>
   </si>
   <si>
-    <t>bv199</t>
-  </si>
-  <si>
-    <t>26/11/2024</t>
-  </si>
-  <si>
-    <t>TS-007854</t>
-  </si>
-  <si>
-    <t>TS-007852</t>
-  </si>
-  <si>
-    <t>TS-008520</t>
-  </si>
-  <si>
-    <t>XEXqJ1</t>
-  </si>
-  <si>
-    <t>05/05/2025</t>
-  </si>
-  <si>
-    <t>04/05/2025</t>
-  </si>
-  <si>
-    <t>TS-007845</t>
-  </si>
-  <si>
-    <t>TS-007894</t>
-  </si>
-  <si>
-    <t>KTS-MOI</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>23/09/2024</t>
-  </si>
-  <si>
-    <t>sondt</t>
-  </si>
-  <si>
-    <t>22/09/2024</t>
-  </si>
-  <si>
-    <t>21/09/2024</t>
-  </si>
-  <si>
-    <t>TS-007871</t>
-  </si>
-  <si>
-    <t>KTS-TAM</t>
-  </si>
-  <si>
-    <t>20/09/2024</t>
-  </si>
-  <si>
-    <t>K.CCDC</t>
-  </si>
-  <si>
-    <t>15/05/2025</t>
-  </si>
-  <si>
-    <t>TS-007502</t>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>31/07/2024</t>
+  </si>
+  <si>
+    <t>18/05/2025</t>
+  </si>
+  <si>
+    <t>TS-007106</t>
+  </si>
+  <si>
+    <t>KTSVT</t>
+  </si>
+  <si>
+    <t>TS-008194</t>
+  </si>
+  <si>
+    <t>KHO_VTYT</t>
+  </si>
+  <si>
+    <t>17/05/2025</t>
+  </si>
+  <si>
+    <t>16/05/2025</t>
+  </si>
+  <si>
+    <t>TS-008195</t>
+  </si>
+  <si>
+    <t>TS-008196</t>
   </si>
 </sst>
 </file>
@@ -918,16 +882,16 @@
         <v>45</v>
       </c>
       <c r="B6" t="s" s="15">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s" s="14">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="D6" t="s" s="23">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s" s="14">
-        <v>75</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>